<commit_message>
Change back to comma
</commit_message>
<xml_diff>
--- a/storage/app/report-template/transaksi.xlsx
+++ b/storage/app/report-template/transaksi.xlsx
@@ -11,8 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$Q$2</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$Q$2</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$V$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$V$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$V$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Tanggal</t>
   </si>
@@ -72,6 +73,21 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
   </si>
 </sst>
 </file>
@@ -260,23 +276,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="10" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="42.234693877551"/>
+    <col collapsed="false" hidden="false" max="22" min="13" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,9 +349,24 @@
       <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q2"/>
+  <autoFilter ref="A1:V2"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
change ukuran to tipe
</commit_message>
<xml_diff>
--- a/storage/app/report-template/transaksi.xlsx
+++ b/storage/app/report-template/transaksi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farizhermawan/other/jmp-tracking-ho-be/storage/app/report-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D3C6EF-7B6B-CC4C-BE66-4DC39164B7C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944E7712-1381-0D4A-9707-6084EEE13411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>Ukuran</t>
+    <t>Tipe</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,8 +157,9 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +545,7 @@
   <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -553,7 +554,7 @@
     <col min="2" max="2" width="14.33203125"/>
     <col min="3" max="4" width="14.1640625"/>
     <col min="5" max="5" width="16.1640625"/>
-    <col min="6" max="6" width="9.83203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="24.6640625"/>
     <col min="8" max="8" width="21.83203125"/>
     <col min="9" max="10" width="20.83203125"/>
@@ -579,7 +580,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">

</xml_diff>

<commit_message>
Add itruck in Transaction
</commit_message>
<xml_diff>
--- a/storage/app/report-template/transaksi.xlsx
+++ b/storage/app/report-template/transaksi.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farizhermawan/other/jmp-trucking-ho-be/storage/app/report-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD35AF8A-245C-9448-9433-DB325714F961}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8637A472-023F-D340-9259-F9DB99D41A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$Z$2</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="0">Sheet1!$A$1:$Z$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$AA$2</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">Sheet1!$A$1:$AA$2</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Tanggal</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Depo MT</t>
+  </si>
+  <si>
+    <t>I-Truck</t>
   </si>
 </sst>
 </file>
@@ -551,32 +554,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.1640625"/>
     <col min="2" max="2" width="14.33203125"/>
-    <col min="3" max="4" width="14.1640625"/>
-    <col min="5" max="5" width="16.1640625"/>
-    <col min="6" max="6" width="10.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21" style="4" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625"/>
-    <col min="9" max="9" width="23.1640625" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125"/>
-    <col min="12" max="13" width="20.83203125"/>
-    <col min="14" max="15" width="21.33203125"/>
-    <col min="16" max="16" width="42.1640625"/>
-    <col min="17" max="26" width="21.33203125"/>
-    <col min="27" max="1029" width="13.6640625"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="5" width="14.1640625"/>
+    <col min="6" max="6" width="16.1640625"/>
+    <col min="7" max="7" width="10.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625"/>
+    <col min="10" max="10" width="23.1640625" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125"/>
+    <col min="13" max="14" width="20.83203125"/>
+    <col min="15" max="16" width="21.33203125"/>
+    <col min="17" max="17" width="42.1640625"/>
+    <col min="18" max="27" width="21.33203125"/>
+    <col min="28" max="1030" width="13.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,80 +588,83 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="R1" s="3">
         <v>1</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AA2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>